<commit_message>
Actualización automática de noticias - 2026-01-10
</commit_message>
<xml_diff>
--- a/data/noticias.xlsx
+++ b/data/noticias.xlsx
@@ -1,88 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
-    <t>titulo</t>
-  </si>
-  <si>
-    <t>fuente</t>
-  </si>
-  <si>
-    <t>ciudad</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>resumen</t>
-  </si>
-  <si>
-    <t>2026-01-09</t>
-  </si>
-  <si>
-    <t>El particular castigo de Policía en Barranquilla a un grupo de jóvenes quedó en video: “El cuerpo sufre”</t>
-  </si>
-  <si>
-    <t>Infobae</t>
-  </si>
-  <si>
-    <t>Barranquilla</t>
-  </si>
-  <si>
-    <t>https://www.infobae.com/colombia/2026/01/09/el-particular-castigo-de-policia-en-barranquilla-a-un-grupo-de-jovenes-quedo-en-video-el-cuerpo-sufre/</t>
-  </si>
-  <si>
-    <t>PorPaula Naranjo</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -97,41 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -419,57 +420,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>fecha</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>titulo</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>fuente</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ciudad</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>resumen</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>El particular castigo de Policía en Barranquilla a un grupo de jóvenes quedó en video: “El cuerpo sufre”</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Infobae</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://www.infobae.com/colombia/2026/01/09/el-particular-castigo-de-policia-en-barranquilla-a-un-grupo-de-jovenes-quedo-en-video-el-cuerpo-sufre/</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>PorPaula Naranjo</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización automática de noticias - 2026-01-12
</commit_message>
<xml_diff>
--- a/data/noticias.xlsx
+++ b/data/noticias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,62 +468,94 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+          <t>PorDahana Ospina</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alerta Bogotá</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>2026-01-09</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>El particular castigo de Policía en Barranquilla a un grupo de jóvenes quedó en video: “El cuerpo sufre”</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Infobae</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Barranquilla</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>https://www.infobae.com/colombia/2026/01/09/el-particular-castigo-de-policia-en-barranquilla-a-un-grupo-de-jovenes-quedo-en-video-el-cuerpo-sufre/</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>PorPaula Naranjo</t>
         </is>

</xml_diff>

<commit_message>
Actualización automática de noticias - 2026-01-13
</commit_message>
<xml_diff>
--- a/data/noticias.xlsx
+++ b/data/noticias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,94 +468,186 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Infobae</t>
+          <t>Alerta Bogotá</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>PorDahana Ospina</t>
-        </is>
-      </c>
+          <t>https://www.alertabogota.com/noticias/local</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+          <t>PorJuan Sánchez Romero</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Diario ADN</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Sin identificar</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://www.diarioadn.co/seccion/actualidad</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Infobae</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sin identificar</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PorDahana Ospina</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alerta Bogotá</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>2026-01-09</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>El particular castigo de Policía en Barranquilla a un grupo de jóvenes quedó en video: “El cuerpo sufre”</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Infobae</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Barranquilla</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>https://www.infobae.com/colombia/2026/01/09/el-particular-castigo-de-policia-en-barranquilla-a-un-grupo-de-jovenes-quedo-en-video-el-cuerpo-sufre/</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>PorPaula Naranjo</t>
         </is>

</xml_diff>

<commit_message>
Actualización automática de noticias - 2026-01-14
</commit_message>
<xml_diff>
--- a/data/noticias.xlsx
+++ b/data/noticias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,40 +468,44 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Menor que fue secuestrada en el Catatumbo denunció que las disidencias la obligaron a enviar mensaje de terror a otros niños</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>https://www.infobae.com/colombia/2026/01/14/menor-que-fue-secuestrada-en-el-catatumbo-denuncio-que-las-disidencias-la-obligaron-a-enviar-mensaje-de-terror-a-otros-ninos/</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>PorJhon Bernal</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
+          <t>Menor de edad colombiano fue baleado frente a su escuela en Chicago, la familia exige justicia</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -511,17 +515,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
+          <t>https://www.infobae.com/colombia/2026/01/14/menor-de-edad-colombiano-fue-baleado-frente-a-su-escuela-en-chicago-la-familia-exige-justicia/</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>PorJuan Sánchez Romero</t>
+          <t>PorJimmy Nomesqui Rivera</t>
         </is>
       </c>
     </row>
@@ -533,39 +537,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Diario ADN</t>
+          <t>Alerta Bogotá</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.diarioadn.co/seccion/actualidad</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
-        </is>
-      </c>
+          <t>https://www.alertabogota.com/noticias/local</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
+          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -580,74 +580,138 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
+          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>PorDahana Ospina</t>
+          <t>PorJuan Sánchez Romero</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Diario ADN</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+          <t>https://www.diarioadn.co/seccion/actualidad</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Infobae</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sin identificar</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>PorDahana Ospina</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alerta Bogotá</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>2026-01-09</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>El particular castigo de Policía en Barranquilla a un grupo de jóvenes quedó en video: “El cuerpo sufre”</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Infobae</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Barranquilla</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>https://www.infobae.com/colombia/2026/01/09/el-particular-castigo-de-policia-en-barranquilla-a-un-grupo-de-jovenes-quedo-en-video-el-cuerpo-sufre/</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>PorPaula Naranjo</t>
         </is>

</xml_diff>

<commit_message>
Actualización automática de noticias - 2026-01-15
</commit_message>
<xml_diff>
--- a/data/noticias.xlsx
+++ b/data/noticias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,12 +468,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Menor que fue secuestrada en el Catatumbo denunció que las disidencias la obligaron a enviar mensaje de terror a otros niños</t>
+          <t>La caída del “capo dei capi” de la Cosa Nostra: de una infancia dura al líder más temido de la mafia siciliana</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -488,24 +488,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/menor-que-fue-secuestrada-en-el-catatumbo-denuncio-que-las-disidencias-la-obligaron-a-enviar-mensaje-de-terror-a-otros-ninos/</t>
+          <t>https://www.infobae.com/historias/2026/01/15/la-caida-del-capo-dei-capi-de-la-cosa-nostra-de-una-infancia-dura-al-lider-mas-temido-de-la-mafia-siciliana/</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>PorJhon Bernal</t>
+          <t>PorGabriela Cicero</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Menor de edad colombiano fue baleado frente a su escuela en Chicago, la familia exige justicia</t>
+          <t>El desplome de los colegios privados en Bogotá no se detiene: 35 cierran sus puertas para 2026</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -515,44 +515,44 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/menor-de-edad-colombiano-fue-baleado-frente-a-su-escuela-en-chicago-la-familia-exige-justicia/</t>
+          <t>https://www.infobae.com/colombia/2026/01/14/el-desplome-de-los-colegios-privados-en-bogota-no-se-detiene-35-cierran-sus-puertas-para-2026/</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>PorJimmy Nomesqui Rivera</t>
+          <t>PorDaniella Mazo González</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Menor de edad colombiana tardó seis años para reencontrarse con su mamá en España, pero murió en grave accidente de tránsito</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local</t>
+          <t>https://www.infobae.com/colombia/2026/01/15/menor-de-edad-colombiana-tardo-seis-anos-para-reencontrarse-con-su-mama-en-espana-pero-murio-en-grave-accidente-de-transito/</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -560,12 +560,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
+          <t>Menor que fue secuestrada en el Catatumbo denunció que las disidencias la obligaron a enviar mensaje de terror a otros niños</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -580,138 +580,230 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
+          <t>https://www.infobae.com/colombia/2026/01/14/menor-que-fue-secuestrada-en-el-catatumbo-denuncio-que-las-disidencias-la-obligaron-a-enviar-mensaje-de-terror-a-otros-ninos/</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>PorJuan Sánchez Romero</t>
+          <t>PorJhon Bernal</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
+          <t>Menor de edad colombiano fue baleado frente a su escuela en Chicago, la familia exige justicia</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Diario ADN</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.diarioadn.co/seccion/actualidad</t>
+          <t>https://www.infobae.com/colombia/2026/01/14/menor-de-edad-colombiano-fue-baleado-frente-a-su-escuela-en-chicago-la-familia-exige-justicia/</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
+          <t>PorJimmy Nomesqui Rivera</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Infobae</t>
+          <t>Alerta Bogotá</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>PorDahana Ospina</t>
-        </is>
-      </c>
+          <t>https://www.alertabogota.com/noticias/local</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+          <t>PorJuan Sánchez Romero</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Diario ADN</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Sin identificar</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://www.diarioadn.co/seccion/actualidad</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Infobae</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Sin identificar</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>PorDahana Ospina</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alerta Bogotá</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>2026-01-09</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>El particular castigo de Policía en Barranquilla a un grupo de jóvenes quedó en video: “El cuerpo sufre”</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Infobae</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Barranquilla</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>https://www.infobae.com/colombia/2026/01/09/el-particular-castigo-de-policia-en-barranquilla-a-un-grupo-de-jovenes-quedo-en-video-el-cuerpo-sufre/</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>PorPaula Naranjo</t>
         </is>

</xml_diff>

<commit_message>
Actualización automática de noticias - 2026-01-16
</commit_message>
<xml_diff>
--- a/data/noticias.xlsx
+++ b/data/noticias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,17 +468,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>La caída del “capo dei capi” de la Cosa Nostra: de una infancia dura al líder más temido de la mafia siciliana</t>
+          <t>Por qué tantas personas de 30 siguen actuando como adolescentes al elegir pareja, según expertos en comportamiento</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Infobae</t>
+          <t>Diario ADN</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -488,44 +488,44 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/historias/2026/01/15/la-caida-del-capo-dei-capi-de-la-cosa-nostra-de-una-infancia-dura-al-lider-mas-temido-de-la-mafia-siciliana/</t>
+          <t>https://www.diarioadn.co/seccion/vida</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>PorGabriela Cicero</t>
+          <t>Afirman que la madurez emocional no llega sola con los años sino que se construye.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>El desplome de los colegios privados en Bogotá no se detiene: 35 cierran sus puertas para 2026</t>
+          <t>Yumbo se pone la camiseta del futuro: lanza Aulas STEAM con inversión histórica de $ 9.500 millones</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Infobae</t>
+          <t>Diario ADN</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/el-desplome-de-los-colegios-privados-en-bogota-no-se-detiene-35-cierran-sus-puertas-para-2026/</t>
+          <t>https://www.diarioadn.co/seccion/regiones</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>PorDaniella Mazo González</t>
+          <t>Iniciativa busca impactar a más de 10.400 estudiantes</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Menor de edad colombiana tardó seis años para reencontrarse con su mamá en España, pero murió en grave accidente de tránsito</t>
+          <t>La caída del “capo dei capi” de la Cosa Nostra: de una infancia dura al líder más temido de la mafia siciliana</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -547,25 +547,29 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/15/menor-de-edad-colombiana-tardo-seis-anos-para-reencontrarse-con-su-mama-en-espana-pero-murio-en-grave-accidente-de-transito/</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+          <t>https://www.infobae.com/historias/2026/01/15/la-caida-del-capo-dei-capi-de-la-cosa-nostra-de-una-infancia-dura-al-lider-mas-temido-de-la-mafia-siciliana/</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>PorGabriela Cicero</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Menor que fue secuestrada en el Catatumbo denunció que las disidencias la obligaron a enviar mensaje de terror a otros niños</t>
+          <t>El desplome de los colegios privados en Bogotá no se detiene: 35 cierran sus puertas para 2026</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -575,29 +579,29 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/menor-que-fue-secuestrada-en-el-catatumbo-denuncio-que-las-disidencias-la-obligaron-a-enviar-mensaje-de-terror-a-otros-ninos/</t>
+          <t>https://www.infobae.com/colombia/2026/01/14/el-desplome-de-los-colegios-privados-en-bogota-no-se-detiene-35-cierran-sus-puertas-para-2026/</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>PorJhon Bernal</t>
+          <t>PorDaniella Mazo González</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Menor de edad colombiano fue baleado frente a su escuela en Chicago, la familia exige justicia</t>
+          <t>Menor de edad colombiana tardó seis años para reencontrarse con su mamá en España, pero murió en grave accidente de tránsito</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -612,52 +616,52 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/menor-de-edad-colombiano-fue-baleado-frente-a-su-escuela-en-chicago-la-familia-exige-justicia/</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>PorJimmy Nomesqui Rivera</t>
-        </is>
-      </c>
+          <t>https://www.infobae.com/colombia/2026/01/15/menor-de-edad-colombiana-tardo-seis-anos-para-reencontrarse-con-su-mama-en-espana-pero-murio-en-grave-accidente-de-transito/</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Menor que fue secuestrada en el Catatumbo denunció que las disidencias la obligaron a enviar mensaje de terror a otros niños</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>https://www.infobae.com/colombia/2026/01/14/menor-que-fue-secuestrada-en-el-catatumbo-denuncio-que-las-disidencias-la-obligaron-a-enviar-mensaje-de-terror-a-otros-ninos/</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>PorJhon Bernal</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
+          <t>Menor de edad colombiano fue baleado frente a su escuela en Chicago, la familia exige justicia</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -667,17 +671,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
+          <t>https://www.infobae.com/colombia/2026/01/14/menor-de-edad-colombiano-fue-baleado-frente-a-su-escuela-en-chicago-la-familia-exige-justicia/</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>PorJuan Sánchez Romero</t>
+          <t>PorJimmy Nomesqui Rivera</t>
         </is>
       </c>
     </row>
@@ -689,39 +693,35 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Diario ADN</t>
+          <t>Alerta Bogotá</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.diarioadn.co/seccion/actualidad</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
-        </is>
-      </c>
+          <t>https://www.alertabogota.com/noticias/local</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
+          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -736,74 +736,138 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
+          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>PorDahana Ospina</t>
+          <t>PorJuan Sánchez Romero</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Diario ADN</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+          <t>https://www.diarioadn.co/seccion/actualidad</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Infobae</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Sin identificar</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>PorDahana Ospina</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alerta Bogotá</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>2026-01-09</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>El particular castigo de Policía en Barranquilla a un grupo de jóvenes quedó en video: “El cuerpo sufre”</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>Infobae</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Barranquilla</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>https://www.infobae.com/colombia/2026/01/09/el-particular-castigo-de-policia-en-barranquilla-a-un-grupo-de-jovenes-quedo-en-video-el-cuerpo-sufre/</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>PorPaula Naranjo</t>
         </is>

</xml_diff>

<commit_message>
Actualización automática de noticias - 2026-01-17
</commit_message>
<xml_diff>
--- a/data/noticias.xlsx
+++ b/data/noticias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,32 +468,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Por qué tantas personas de 30 siguen actuando como adolescentes al elegir pareja, según expertos en comportamiento</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Diario ADN</t>
+          <t>Pulzo</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.diarioadn.co/seccion/vida</t>
+          <t>https://www.pulzo.com/nacion/que-trata-cambio-estructural-educacion-colombia-por-giro-pae-PP4995431</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Afirman que la madurez emocional no llega sola con los años sino que se construye.</t>
+          <t>Anuncian cambio estructural para educación en Colombia: nueva resolución toca a 550.000 niños</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Yumbo se pone la camiseta del futuro: lanza Aulas STEAM con inversión histórica de $ 9.500 millones</t>
+          <t>Por qué tantas personas de 30 siguen actuando como adolescentes al elegir pareja, según expertos en comportamiento</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -520,29 +520,29 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.diarioadn.co/seccion/regiones</t>
+          <t>https://www.diarioadn.co/seccion/vida</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Iniciativa busca impactar a más de 10.400 estudiantes</t>
+          <t>Afirman que la madurez emocional no llega sola con los años sino que se construye.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>La caída del “capo dei capi” de la Cosa Nostra: de una infancia dura al líder más temido de la mafia siciliana</t>
+          <t>Yumbo se pone la camiseta del futuro: lanza Aulas STEAM con inversión histórica de $ 9.500 millones</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Infobae</t>
+          <t>Diario ADN</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -552,12 +552,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/historias/2026/01/15/la-caida-del-capo-dei-capi-de-la-cosa-nostra-de-una-infancia-dura-al-lider-mas-temido-de-la-mafia-siciliana/</t>
+          <t>https://www.diarioadn.co/seccion/regiones</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>PorGabriela Cicero</t>
+          <t>Iniciativa busca impactar a más de 10.400 estudiantes</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>El desplome de los colegios privados en Bogotá no se detiene: 35 cierran sus puertas para 2026</t>
+          <t>La caída del “capo dei capi” de la Cosa Nostra: de una infancia dura al líder más temido de la mafia siciliana</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -579,17 +579,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/el-desplome-de-los-colegios-privados-en-bogota-no-se-detiene-35-cierran-sus-puertas-para-2026/</t>
+          <t>https://www.infobae.com/historias/2026/01/15/la-caida-del-capo-dei-capi-de-la-cosa-nostra-de-una-infancia-dura-al-lider-mas-temido-de-la-mafia-siciliana/</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>PorDaniella Mazo González</t>
+          <t>PorGabriela Cicero</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Menor de edad colombiana tardó seis años para reencontrarse con su mamá en España, pero murió en grave accidente de tránsito</t>
+          <t>El desplome de los colegios privados en Bogotá no se detiene: 35 cierran sus puertas para 2026</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -611,25 +611,29 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/15/menor-de-edad-colombiana-tardo-seis-anos-para-reencontrarse-con-su-mama-en-espana-pero-murio-en-grave-accidente-de-transito/</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>https://www.infobae.com/colombia/2026/01/14/el-desplome-de-los-colegios-privados-en-bogota-no-se-detiene-35-cierran-sus-puertas-para-2026/</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PorDaniella Mazo González</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Menor que fue secuestrada en el Catatumbo denunció que las disidencias la obligaron a enviar mensaje de terror a otros niños</t>
+          <t>Menor de edad colombiana tardó seis años para reencontrarse con su mamá en España, pero murió en grave accidente de tránsito</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -639,19 +643,15 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/menor-que-fue-secuestrada-en-el-catatumbo-denuncio-que-las-disidencias-la-obligaron-a-enviar-mensaje-de-terror-a-otros-ninos/</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>PorJhon Bernal</t>
-        </is>
-      </c>
+          <t>https://www.infobae.com/colombia/2026/01/15/menor-de-edad-colombiana-tardo-seis-anos-para-reencontrarse-con-su-mama-en-espana-pero-murio-en-grave-accidente-de-transito/</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Menor de edad colombiano fue baleado frente a su escuela en Chicago, la familia exige justicia</t>
+          <t>Menor que fue secuestrada en el Catatumbo denunció que las disidencias la obligaron a enviar mensaje de terror a otros niños</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -671,47 +671,51 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/menor-de-edad-colombiano-fue-baleado-frente-a-su-escuela-en-chicago-la-familia-exige-justicia/</t>
+          <t>https://www.infobae.com/colombia/2026/01/14/menor-que-fue-secuestrada-en-el-catatumbo-denuncio-que-las-disidencias-la-obligaron-a-enviar-mensaje-de-terror-a-otros-ninos/</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>PorJimmy Nomesqui Rivera</t>
+          <t>PorJhon Bernal</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Menor de edad colombiano fue baleado frente a su escuela en Chicago, la familia exige justicia</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+          <t>https://www.infobae.com/colombia/2026/01/14/menor-de-edad-colombiano-fue-baleado-frente-a-su-escuela-en-chicago-la-familia-exige-justicia/</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>PorJimmy Nomesqui Rivera</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -721,29 +725,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Infobae</t>
+          <t>Alerta Bogotá</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>PorJuan Sánchez Romero</t>
-        </is>
-      </c>
+          <t>https://www.alertabogota.com/noticias/local</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -753,12 +753,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
+          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Diario ADN</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -768,29 +768,29 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.diarioadn.co/seccion/actualidad</t>
+          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
+          <t>PorJuan Sánchez Romero</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
+          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Infobae</t>
+          <t>Diario ADN</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -800,74 +800,106 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
+          <t>https://www.diarioadn.co/seccion/actualidad</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>PorDahana Ospina</t>
+          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+          <t>PorDahana Ospina</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alerta Bogotá</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>2026-01-09</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>El particular castigo de Policía en Barranquilla a un grupo de jóvenes quedó en video: “El cuerpo sufre”</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Infobae</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Barranquilla</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>https://www.infobae.com/colombia/2026/01/09/el-particular-castigo-de-policia-en-barranquilla-a-un-grupo-de-jovenes-quedo-en-video-el-cuerpo-sufre/</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>PorPaula Naranjo</t>
         </is>

</xml_diff>

<commit_message>
Actualización automática de noticias - 2026-01-18
</commit_message>
<xml_diff>
--- a/data/noticias.xlsx
+++ b/data/noticias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,64 +468,60 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Este es el calendario de vacaciones y recesos en colegios públicos de Bogotá en 2026, prográmese</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Pulzo</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.pulzo.com/nacion/que-trata-cambio-estructural-educacion-colombia-por-giro-pae-PP4995431</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Anuncian cambio estructural para educación en Colombia: nueva resolución toca a 550.000 niños</t>
-        </is>
-      </c>
+          <t>https://www.infobae.com/colombia/2026/01/17/este-es-el-calendario-de-vacaciones-y-recesos-en-colegios-publicos-de-bogota-en-2026-programese/</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Por qué tantas personas de 30 siguen actuando como adolescentes al elegir pareja, según expertos en comportamiento</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Diario ADN</t>
+          <t>Pulzo</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.diarioadn.co/seccion/vida</t>
+          <t>https://www.pulzo.com/nacion/que-trata-cambio-estructural-educacion-colombia-por-giro-pae-PP4995431</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Afirman que la madurez emocional no llega sola con los años sino que se construye.</t>
+          <t>Anuncian cambio estructural para educación en Colombia: nueva resolución toca a 550.000 niños</t>
         </is>
       </c>
     </row>
@@ -537,7 +533,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Yumbo se pone la camiseta del futuro: lanza Aulas STEAM con inversión histórica de $ 9.500 millones</t>
+          <t>Por qué tantas personas de 30 siguen actuando como adolescentes al elegir pareja, según expertos en comportamiento</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -552,29 +548,29 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.diarioadn.co/seccion/regiones</t>
+          <t>https://www.diarioadn.co/seccion/vida</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Iniciativa busca impactar a más de 10.400 estudiantes</t>
+          <t>Afirman que la madurez emocional no llega sola con los años sino que se construye.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>La caída del “capo dei capi” de la Cosa Nostra: de una infancia dura al líder más temido de la mafia siciliana</t>
+          <t>Yumbo se pone la camiseta del futuro: lanza Aulas STEAM con inversión histórica de $ 9.500 millones</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Infobae</t>
+          <t>Diario ADN</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -584,12 +580,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/historias/2026/01/15/la-caida-del-capo-dei-capi-de-la-cosa-nostra-de-una-infancia-dura-al-lider-mas-temido-de-la-mafia-siciliana/</t>
+          <t>https://www.diarioadn.co/seccion/regiones</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>PorGabriela Cicero</t>
+          <t>Iniciativa busca impactar a más de 10.400 estudiantes</t>
         </is>
       </c>
     </row>
@@ -601,7 +597,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>El desplome de los colegios privados en Bogotá no se detiene: 35 cierran sus puertas para 2026</t>
+          <t>La caída del “capo dei capi” de la Cosa Nostra: de una infancia dura al líder más temido de la mafia siciliana</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -611,17 +607,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/el-desplome-de-los-colegios-privados-en-bogota-no-se-detiene-35-cierran-sus-puertas-para-2026/</t>
+          <t>https://www.infobae.com/historias/2026/01/15/la-caida-del-capo-dei-capi-de-la-cosa-nostra-de-una-infancia-dura-al-lider-mas-temido-de-la-mafia-siciliana/</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>PorDaniella Mazo González</t>
+          <t>PorGabriela Cicero</t>
         </is>
       </c>
     </row>
@@ -633,7 +629,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Menor de edad colombiana tardó seis años para reencontrarse con su mamá en España, pero murió en grave accidente de tránsito</t>
+          <t>El desplome de los colegios privados en Bogotá no se detiene: 35 cierran sus puertas para 2026</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -643,25 +639,29 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/15/menor-de-edad-colombiana-tardo-seis-anos-para-reencontrarse-con-su-mama-en-espana-pero-murio-en-grave-accidente-de-transito/</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>https://www.infobae.com/colombia/2026/01/14/el-desplome-de-los-colegios-privados-en-bogota-no-se-detiene-35-cierran-sus-puertas-para-2026/</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>PorDaniella Mazo González</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Menor que fue secuestrada en el Catatumbo denunció que las disidencias la obligaron a enviar mensaje de terror a otros niños</t>
+          <t>Menor de edad colombiana tardó seis años para reencontrarse con su mamá en España, pero murió en grave accidente de tránsito</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -671,19 +671,15 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/menor-que-fue-secuestrada-en-el-catatumbo-denuncio-que-las-disidencias-la-obligaron-a-enviar-mensaje-de-terror-a-otros-ninos/</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>PorJhon Bernal</t>
-        </is>
-      </c>
+          <t>https://www.infobae.com/colombia/2026/01/15/menor-de-edad-colombiana-tardo-seis-anos-para-reencontrarse-con-su-mama-en-espana-pero-murio-en-grave-accidente-de-transito/</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -693,7 +689,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Menor de edad colombiano fue baleado frente a su escuela en Chicago, la familia exige justicia</t>
+          <t>Menor que fue secuestrada en el Catatumbo denunció que las disidencias la obligaron a enviar mensaje de terror a otros niños</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -703,47 +699,51 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/14/menor-de-edad-colombiano-fue-baleado-frente-a-su-escuela-en-chicago-la-familia-exige-justicia/</t>
+          <t>https://www.infobae.com/colombia/2026/01/14/menor-que-fue-secuestrada-en-el-catatumbo-denuncio-que-las-disidencias-la-obligaron-a-enviar-mensaje-de-terror-a-otros-ninos/</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>PorJimmy Nomesqui Rivera</t>
+          <t>PorJhon Bernal</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Menor de edad colombiano fue baleado frente a su escuela en Chicago, la familia exige justicia</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
+          <t>https://www.infobae.com/colombia/2026/01/14/menor-de-edad-colombiano-fue-baleado-frente-a-su-escuela-en-chicago-la-familia-exige-justicia/</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>PorJimmy Nomesqui Rivera</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -753,29 +753,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Infobae</t>
+          <t>Alerta Bogotá</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Sin identificar</t>
+          <t>Bogotá</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>PorJuan Sánchez Romero</t>
-        </is>
-      </c>
+          <t>https://www.alertabogota.com/noticias/local</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -785,12 +781,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
+          <t>Treinta niños quedaron sin aulas en zona rural de Nechí, Antioquia: incendio incineró la única escuela de un caserío</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Diario ADN</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -800,29 +796,29 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.diarioadn.co/seccion/actualidad</t>
+          <t>https://www.infobae.com/colombia/2026/01/13/treinta-ninos-quedaron-sin-aulas-en-zona-rural-de-nechi-antioquia-incendio-incinero-la-unica-escuela-de-un-caserio/</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
+          <t>PorJuan Sánchez Romero</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
+          <t>Tres estudiantes resultan heridos tras caer desde un bus de dos niveles; autoridades investigan</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Infobae</t>
+          <t>Diario ADN</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -832,74 +828,106 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
+          <t>https://www.diarioadn.co/seccion/actualidad</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>PorDahana Ospina</t>
+          <t>Los menores, de 13 y 14 años, tuvieron que ser hospitalizados.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+          <t>Madre denuncia a Karina García por grabar a su hija menor de edad sin autorización durante una transmisión en vivo</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Alerta Bogotá</t>
+          <t>Infobae</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Sin identificar</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+          <t>https://www.infobae.com/colombia/2026/01/12/madre-denuncia-a-karina-garcia-por-grabar-a-su-hija-menor-de-edad-sin-autorizacion-durante-una-transmision-en-vivo/</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+          <t>PorDahana Ospina</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Estudiantes respiran con el aumento del pasaje de TransMilenio: no tendrán que gastarse lo del almuerzo</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alerta Bogotá</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Bogotá</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://www.alertabogota.com/noticias/local/estudiantes-respiran-con-el-aumento-del-pasaje-de-transmilenio-no-tendran-que-gastarse-lo-del-almuerzo</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>El incremento en el pasaje no será una barrera para que los estudiantes continúen asistiendo a clases.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>2026-01-09</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>El particular castigo de Policía en Barranquilla a un grupo de jóvenes quedó en video: “El cuerpo sufre”</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Infobae</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Barranquilla</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>https://www.infobae.com/colombia/2026/01/09/el-particular-castigo-de-policia-en-barranquilla-a-un-grupo-de-jovenes-quedo-en-video-el-cuerpo-sufre/</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>PorPaula Naranjo</t>
         </is>

</xml_diff>